<commit_message>
[improvements] - allow screenshots to be enhanced with caption-related System variables:   - [`nexial.screenshot.position`]: specify where the caption should be placed.   - [`nexial.screenshot.alpha`]: specify the transparency of the rendered caption text.   - [`nexial.screenshot.wrap`]: specify if the rendered caption text should be rendered as contiguous text or not.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/image-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/image-showcase.data.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11104"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9644EC99-2B87-1149-96F9-FC1A36E9F4D0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27D069D-F1F3-DE49-93F2-7B06D413BDF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10880" yWindow="16380" windowWidth="33600" windowHeight="15100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6080" yWindow="19960" windowWidth="33600" windowHeight="15100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
     <sheet name="diff-prep" sheetId="3" r:id="rId2"/>
     <sheet name="diff" sheetId="4" r:id="rId3"/>
+    <sheet name="screenshots" sheetId="5" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -38,10 +39,18 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -51,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>true</t>
   </si>
@@ -126,6 +135,14 @@
   </si>
   <si>
     <t>80000</t>
+  </si>
+  <si>
+    <t>nexial.screenshot.caption</t>
+  </si>
+  <si>
+    <t>$(execution|script|name)
+$(execution|scenario|name) - $(execution|step|index)
+Captured on: $(sysdate|now|yyyy/MM/dd HH:mm:ss)</t>
   </si>
 </sst>
 </file>
@@ -258,7 +275,72 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -843,21 +925,21 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="19" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="18" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -870,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1700CE5F-11B4-0E40-8F44-4E925DF2E821}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -962,21 +1044,21 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1093,6 +1175,96 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="7" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="5">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A586D4B7-D7DB-084A-9A31-4EA1129B0CAA}">
+  <dimension ref="A1:AAA10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="27.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="71" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703" ht="54">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703">
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703">
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703">
+      <c r="B4" s="7"/>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703">
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703">
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703">
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703">
+      <c r="HA10" s="4"/>
+      <c r="AAA10" s="5"/>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>

</xml_diff>

<commit_message>
[improvement] - [`nexial.screenshot.noBackground`]: specify if complementary background color should be rendered along with the caption. Default is `true`.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/image-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/image-showcase.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27D069D-F1F3-DE49-93F2-7B06D413BDF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78C0B70-A2FF-2F46-9921-F21E7020A584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="19960" windowWidth="33600" windowHeight="15100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6280" yWindow="-21140" windowWidth="18200" windowHeight="21140" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>true</t>
   </si>
@@ -143,6 +143,9 @@
     <t>$(execution|script|name)
 $(execution|scenario|name) - $(execution|step|index)
 Captured on: $(sysdate|now|yyyy/MM/dd HH:mm:ss)</t>
+  </si>
+  <si>
+    <t>// nexial.browser</t>
   </si>
 </sst>
 </file>
@@ -1202,14 +1205,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A586D4B7-D7DB-084A-9A31-4EA1129B0CAA}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="150" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="71" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="22.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="76.5" style="2" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
@@ -1226,6 +1229,12 @@
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
@@ -1251,10 +1260,12 @@
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
+      <c r="B8" s="7"/>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
-    <row r="9" spans="1:703">
+    <row r="9" spans="1:703" ht="22" customHeight="1">
+      <c r="B9" s="7"/>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>

</xml_diff>

<commit_message>
[image] - code fix to properly state the need for Oracle JDK when processing JPG images. - code refactoring to keep image processing code in one class.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/image-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/image-showcase.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78C0B70-A2FF-2F46-9921-F21E7020A584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E344B2D-0867-F544-8CED-EC369F0375A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="-21140" windowWidth="18200" windowHeight="21140" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="14860" windowWidth="18200" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>true</t>
   </si>
@@ -828,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA10"/>
+  <dimension ref="A1:AAA6"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -874,56 +874,16 @@
       <c r="AAA3" s="6"/>
     </row>
     <row r="4" spans="1:703">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
-    </row>
-    <row r="7" spans="1:703">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="HA7" s="4"/>
-      <c r="AAA7" s="5"/>
-    </row>
-    <row r="8" spans="1:703">
-      <c r="HA8" s="4"/>
-      <c r="AAA8" s="5"/>
-    </row>
-    <row r="9" spans="1:703">
-      <c r="HA9" s="4"/>
-      <c r="AAA9" s="5"/>
-    </row>
-    <row r="10" spans="1:703">
-      <c r="HA10" s="4"/>
-      <c r="AAA10" s="5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
@@ -956,7 +916,7 @@
   <dimension ref="A1:AAA10"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1205,7 +1165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A586D4B7-D7DB-084A-9A31-4EA1129B0CAA}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="150" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="133" zoomScaleNormal="150" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[web] - [metrics]: minor type fix
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/image-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/image-showcase.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E344B2D-0867-F544-8CED-EC369F0375A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50ACECF-3835-E244-92F8-0D4633C2BD62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="14860" windowWidth="18200" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24340" yWindow="6100" windowWidth="21940" windowHeight="16600" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>true</t>
   </si>
@@ -146,6 +146,11 @@
   </si>
   <si>
     <t>// nexial.browser</t>
+  </si>
+  <si>
+    <t>Search for "Sire m7"
+$(execution|scenario|name) - Step $(execution|step|index)
+Posted on $(sysdate|now|yyyy/MM/dd HH:mm:ss)</t>
   </si>
 </sst>
 </file>
@@ -830,7 +835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1165,13 +1170,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A586D4B7-D7DB-084A-9A31-4EA1129B0CAA}">
   <dimension ref="A1:AAA10"/>
   <sheetViews>
-    <sheetView zoomScale="133" zoomScaleNormal="150" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="150" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="76.5" style="2" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
@@ -1202,8 +1207,13 @@
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
-    <row r="4" spans="1:703">
-      <c r="B4" s="7"/>
+    <row r="4" spans="1:703" ht="54">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>

</xml_diff>